<commit_message>
Funcionando con normalidad: TODO - Archivo de configuración para la codificación de cada factura - Búsqueda de clientes y facturas - Resumen a partir de fechas
</commit_message>
<xml_diff>
--- a/facturas/trimestral.xlsx
+++ b/facturas/trimestral.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,44 +466,40 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>IVA</t>
+          <t>IVA %</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Descuento</t>
+          <t xml:space="preserve">Descuento % </t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Total facturado €</t>
+          <t>Total facturado €(Impuestos y descuentos incluidos</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FASE DE PRUEBAS</t>
+          <t>A200001</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Luis Zurita Herrera</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>74666101M</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Clientes contado </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -515,39 +511,39 @@
         <v>32</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J3" t="n">
-        <v>32</v>
+        <v>31.62</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FASE DE PRUEBAS 3</t>
+          <t>A200002</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2020-09-01</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">asdfasdf asdfasdf asdfasdf </t>
+          <t>Luis Zurita Herrera</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>12345678F</t>
+          <t>74666101M</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -556,42 +552,42 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>97.28</v>
+        <v>64</v>
       </c>
       <c r="H4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>101.1712</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FASE DE PRUEBAS 2</t>
+          <t>A200003</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>otro molomngo</t>
+          <t>Luis Zurita Herrera</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>asdff444</t>
+          <t>74666101M</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -603,39 +599,35 @@
         <v>32</v>
       </c>
       <c r="H5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J5" t="n">
-        <v>33.28</v>
+        <v>27.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FASE DE PRUEBAS</t>
+          <t>A200004</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Luis Zurita Herrera</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>74666101M</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Clientes contado </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -644,7 +636,7 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -653,33 +645,29 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>64</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>0'''ierdas</t>
+          <t>A200005</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2020-09-01</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>otro molomngo</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>asdff444</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Clientes contado </t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -688,42 +676,38 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>97.28</v>
+        <v>64</v>
       </c>
       <c r="H7" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>101.1712</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> asdf asdf0'''ierdas</t>
+          <t>A200006</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2020-09-01</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>otro molomngo</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>asdff444</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Clientes contado </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -732,91 +716,83 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>161.28</v>
+        <v>32</v>
       </c>
       <c r="H8" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>167.7312</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>factura llena de mierdas</t>
+          <t>A200007</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2020-09-01</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">asdfasdf asdfasdf asdfasdf </t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>12345678F</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Clientes contado </t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Sesión de Fisioterapia</t>
+          <t>Sesión de Acupuntura</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>32</v>
+        <v>81.59</v>
       </c>
       <c r="H9" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J9" t="n">
-        <v>33.28</v>
+        <v>76.02</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>fdgfgfg  DE PRUEBAS</t>
+          <t>A200008</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">asdfasdf asdfasdf asdfasdf </t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>12345678F</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Clientes contado </t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Sesión de Fisioterapia</t>
+          <t>ffdfasdfdasfdsaf</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -835,36 +811,32 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>fdgfgfg  gggggDE PRUEBAS</t>
+          <t>A200009</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">asdfasdf asdfasdf asdfasdf </t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>12345678F</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Clientes contado </t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Sesión de Fisioterapia</t>
+          <t>acu</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -873,77 +845,73 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>fdgfgfg  glllllggggDE PRUEBAS</t>
+          <t>A200010</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">asdfasdf asdfasdf asdfasdf </t>
+          <t>Luis Zurita Herrera</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>12345678F</t>
+          <t>74666101M</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Sesión de Fisioterapia</t>
+          <t>acu</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J12" t="n">
-        <v>32</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>'¡DE PRUEBAS</t>
+          <t>A200011</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">asdfasdf asdfasdf asdfasdf </t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>12345678F</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Clientes contado </t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>2020-09-06</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -952,7 +920,7 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -961,50 +929,6 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>56uu6j6u gggDE PRUEBAS</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>2020-09-05</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">asdfasdf asdfasdf asdfasdf </t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>12345678F</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2020-09-05</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Sesión de Fisioterapia</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
-        <v>32</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Programa funcionando y exporta datos correctamente
</commit_message>
<xml_diff>
--- a/facturas/trimestral.xlsx
+++ b/facturas/trimestral.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,7 +488,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2020-09-06</t>
+          <t>2020-09-12</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -499,7 +499,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2020-09-06</t>
+          <t>2020-09-12</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -508,16 +508,16 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>32</v>
+        <v>112</v>
       </c>
       <c r="H3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>31.62</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4">
@@ -528,22 +528,18 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2020-09-06</t>
+          <t>2020-09-12</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Luis Zurita Herrera</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>74666101M</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Clientes contado </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2020-09-06</t>
+          <t>2020-09-12</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -552,7 +548,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -561,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>64</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
@@ -572,22 +568,18 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2020-09-06</t>
+          <t>2020-09-12</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Luis Zurita Herrera</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>74666101M</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Clientes contado </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2020-09-06</t>
+          <t>2020-09-12</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -596,16 +588,16 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>27.2</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6">
@@ -616,7 +608,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2020-09-06</t>
+          <t>2020-09-12</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -627,7 +619,7 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2020-09-06</t>
+          <t>2020-09-12</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -636,7 +628,7 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -645,7 +637,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -656,18 +648,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2020-09-06</t>
+          <t>2020-09-12</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Clientes contado </t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
+          <t>luis aslñdkf</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>74666101M</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2020-09-06</t>
+          <t>2020-09-12</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -676,7 +672,7 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -685,7 +681,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>64</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
@@ -696,7 +692,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2020-09-06</t>
+          <t>2020-09-12</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -707,7 +703,7 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2020-09-06</t>
+          <t>2020-09-12</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -716,7 +712,7 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -725,211 +721,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>A200007</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2020-09-06</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Clientes contado </t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2020-09-06</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Sesión de Acupuntura</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>81.59</v>
-      </c>
-      <c r="H9" t="n">
-        <v>21</v>
-      </c>
-      <c r="I9" t="n">
-        <v>23</v>
-      </c>
-      <c r="J9" t="n">
-        <v>76.02</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>A200008</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2020-09-06</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Clientes contado </t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>2020-09-06</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>ffdfasdfdasfdsaf</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
-        <v>32</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>A200009</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2020-09-06</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Clientes contado </t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>2020-09-06</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>acu</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>50</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>A200010</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2020-09-06</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Luis Zurita Herrera</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>74666101M</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2020-09-06</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>acu</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
-        <v>100</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>12</v>
-      </c>
-      <c r="J12" t="n">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>A200011</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2020-09-06</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Clientes contado </t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2020-09-06</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Sesión de Fisioterapia</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>32</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>